<commit_message>
final_sim: Changed launch config file then changed it back after testing the simulator with long pauses on the background process.
</commit_message>
<xml_diff>
--- a/1_final-sim/neural_body/sim_configs/launch_sat_config.xlsx
+++ b/1_final-sim/neural_body/sim_configs/launch_sat_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craig\Documents\Git\neural-body\1_final-sim\neural_body\sim_configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20CC228-B0BA-4604-A74E-4BF0147A4F74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F98D48-06A0-4FD6-B365-80C150D1E0D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimConfig" sheetId="3" r:id="rId1"/>
@@ -321,7 +321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF846D29-C8D2-4A70-A77B-6EE37888FC0B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -352,7 +352,7 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>